<commit_message>
First version of Wheelbase and ODR goes online!
</commit_message>
<xml_diff>
--- a/socvcap.xlsx
+++ b/socvcap.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianpycior/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianpycior/sebasportfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="3260" yWindow="460" windowWidth="22340" windowHeight="15040" tabRatio="500" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Infant Mortality Rate" sheetId="1" r:id="rId1"/>
@@ -1589,11 +1589,12 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="A1:C16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>